<commit_message>
todays work 5th july
</commit_message>
<xml_diff>
--- a/documents/TSAUTOMATIONSAMPLE.xlsx
+++ b/documents/TSAUTOMATIONSAMPLE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NidSample" sheetId="1" state="visible" r:id="rId2"/>
@@ -153,7 +153,7 @@
     <t xml:space="preserve">E-Pan</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/rohit.singh/git/repository1/truth_screen/documents/Multiple_ocr/PAN/companypan-converted.pdf</t>
+    <t xml:space="preserve">/home/rohit.singh/git/repository1/truth_screen/documents/Multiple_ocr/PAN/VF E-PAN (1).pdf</t>
   </si>
   <si>
     <t xml:space="preserve">12</t>
@@ -456,7 +456,7 @@
     <t xml:space="preserve">cowin Link Generate</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/rohit.singh/Downloads/cowinlink.csv</t>
+    <t xml:space="preserve">/home/rohit.singh/Downloads/cowin_links (1).csv</t>
   </si>
   <si>
     <t xml:space="preserve">PEP search</t>
@@ -1719,10 +1719,10 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.62"/>
@@ -1998,10 +1998,10 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.11"/>
@@ -2113,11 +2113,11 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="34.59"/>
@@ -2557,10 +2557,10 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.09"/>
@@ -2667,11 +2667,11 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="31.28"/>
@@ -2907,7 +2907,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.34"/>
@@ -3068,7 +3068,7 @@
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.6"/>
@@ -3390,7 +3390,7 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.28"/>
@@ -3495,7 +3495,7 @@
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>

</xml_diff>